<commit_message>
Distribution channel add for all module excel upload
</commit_message>
<xml_diff>
--- a/assets/samples/discount_actual_sample.xlsx
+++ b/assets/samples/discount_actual_sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\territory_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazenet- User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8EA0EE-915C-4760-9D30-B36E1E243849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808BD3C6-394B-44C3-83CC-B61DBA6D62F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{51D90B15-872F-42ED-81C5-88158AB9F870}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Product division</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>MH01</t>
+  </si>
+  <si>
+    <t>Distribution channel code</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>GO</t>
   </si>
 </sst>
 </file>
@@ -446,7 +455,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEBCFD8E-FE96-4FD9-A287-3F23ED1884EF}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1:I1048576"/>
@@ -458,9 +467,10 @@
     <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,10 +496,13 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -514,11 +527,14 @@
       <c r="H2">
         <v>196</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -543,7 +559,10 @@
       <c r="H3">
         <v>192</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Distribution field add for excel upload in all modules
</commit_message>
<xml_diff>
--- a/assets/samples/discount_actual_sample.xlsx
+++ b/assets/samples/discount_actual_sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\territory_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazenet- User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8EA0EE-915C-4760-9D30-B36E1E243849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808BD3C6-394B-44C3-83CC-B61DBA6D62F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{51D90B15-872F-42ED-81C5-88158AB9F870}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Product division</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>MH01</t>
+  </si>
+  <si>
+    <t>Distribution channel code</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>GO</t>
   </si>
 </sst>
 </file>
@@ -446,7 +455,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEBCFD8E-FE96-4FD9-A287-3F23ED1884EF}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1:I1048576"/>
@@ -458,9 +467,10 @@
     <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,10 +496,13 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -514,11 +527,14 @@
       <c r="H2">
         <v>196</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -543,7 +559,10 @@
       <c r="H3">
         <v>192</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3">
         <v>8</v>
       </c>
     </row>

</xml_diff>